<commit_message>
Get daily reddit data: Tue Jan  7 08:11:00 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_12.xlsx
+++ b/data/collected_data/2025_01_12.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C494"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3287 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1hvlq8c</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Why are my nails lifting :(</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvlq8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1hvlyyw</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newbie question: can cat eye polishes be non gel? </t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hvlyyw/newbie_question_can_cat_eye_polishes_be_non_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1hvls0y</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Has anyone ordered press ons from Glampop?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hvls0y/has_anyone_ordered_press_ons_from_glampop/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1hvlgp9</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Very 1st Attempt at Black french with Butterflies. Thoughts??</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvlgp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1hvlb1w</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Which nail shape elongates my fingers more?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvlb1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1hvju6i</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Gel X Questions/side effects</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hvju6i/gel_x_questionsside_effects/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1hvjr12</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Help— nail is broken and about to fall off!</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g189c3qn5ibe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1hvk5bs</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Made a fun comic-styled 💥Valentine’s Day set(hand painted hearts and stamped words)</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2x0nsr1m9ibe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1hvk19h</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>First time painting my nails what are your thoughts? Essie “second hand, first love”</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0uvrdze8ibe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1hvjc34</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>chrome nails … yay or nay ?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vp5y4zae1ibe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1hvj1my</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Just did them myself for the first time and fixed my weird index finger! 😅</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2rju3ukyhbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1hvj0dc</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Manicure Monday </t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uc8rdyf8yhbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1hviqug</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Any SpyxFamily Fans in here? 🙈</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/suxhfdyovhbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1hvhzuw</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Maybe an odd idea, but… commenters choose my nails!</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hvhzuw/maybe_an_odd_idea_but_commenters_choose_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1hvih0a</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Is it worth it to rent press on nails?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hvih0a/is_it_worth_it_to_rent_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1hvi6df</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>First Time, Full Hand</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bz99tq8eqhbe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1hvhuzc</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternative BIAB brand to Ukrainian Dark pro base </t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://riornails.com/en/catalog/dark/dark_pro_base_16_15_ml/?srsltid=AfmBOop7nSMlV6OoyubiCeJHz3pPOgwvkMYQGARNMxth49-5cx1e0pXo</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1hvhieg</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Ponyo🪼</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wx0wr5cckhbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1hvgu8y</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail girl is amazing </t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvgu8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1hvgu6y</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>In process of growing out real nails :(</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnty97c6ehbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1hvgs8w</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Mooncat's Millennia</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l6gukf6ndhbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1hvgp0w</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Does anyone else have really wide fingernails that you've had since birth?</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hvgp0w/does_anyone_else_have_really_wide_fingernails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1hvghmu</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Just got my nails done</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ln1fzl04bhbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1hvghgv</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Best alternatives?</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hvghgv/best_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1hvg23h</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Is the new growth noticeable?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2n9jw7a7hbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1hvg0s9</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Choosing between nails</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmknbdiy6hbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1hvfxq7</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love this new OPI gel nail color! </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nm990ne86hbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1hvfs5p</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Wishing I could have fancier nails…</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4e0wgdfz4hbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1hvfmg5</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>POSCA markers are great for dating nail polishes.</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mz7ezkn3hbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1hvf42g</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Molten Fire In The Sky 🌋🌉</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvf42g</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1hvetxv</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails 💅 </t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5pftn9f2xgbe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1hveos1</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Free edge breaking</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wnja0qwvgbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1hveben</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>❄️❄️❄️❄️</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hveben</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1hveab6</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Took a break from acrylics, now back at it again with a green set 💚🍏</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hveab6</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1hvdw95</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>LOVE THESE💅🏻</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvdw95</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1hvd6hs</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>What nail shape would make my fingers look longer/thinner?</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvd6hs</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1hvctku</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Wicked inspired nails </t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvctku</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1hvd5tt</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this gel allergy?? </t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvd5tt</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1hvdb8z</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Polygel</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvdb8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1hvd64s</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>My last set of 2024</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4hn5ywpjgbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1hvcwfu</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Absolutely love a French with flair, so classy. Loving my nails and tried a bit of gold for the first time </t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvcwfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1hvcprk</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>First set of 2025 (and second set I've done myself)</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvcprk</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1hvc2kd</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Enjoying the holidays for a little longer ✨🎅🏻🎄</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ysqxv05bgbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1hvbxn6</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Romantic Gothic set</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvbxn6</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1hvbw3y</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>To the user with duck nails - a fix!</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sdwtfuir9gbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1hvblef</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Deep blue &amp; icy jewels 💙🤍</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ua9ox0fi7gbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1hvbhtn</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alexa, play Potential by Summer Walker </t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvbhtn</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1hvbckc</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>🌿 Leafy 🌿</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rinbnyl5gbe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1hvb7g5</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Price of manicure</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hvb7g5/price_of_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1hvb37b</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>I finally tried press on TOE nails</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4gwlullo3gbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1hvb30m</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Painted this mini Irn Bru can to test myself 😮‍💨 My wrists ARE SHAKING from being so strained 🤣🫶🏼</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1ss0vwvm3gbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1hvb1xi</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ACOTAR </t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hvb1xi/acotar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1hvasri</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Help, is it possible to somehow repair these nails?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvasri</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1hvas5q</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Should I shape the rest of my nails more round to match my weird index finger?</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvas5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1hva4d8</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>How can I help my wife?</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hva4d8</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1hvaix5</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>A couple practice sets/practice nails I did over the weekend.</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvaix5</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1hvaaac</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>January</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvaaac</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1hvaa91</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute Pink Nails </t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1eailjqxfbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1hva6o3</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Galactic chrome 🪐</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ro79uu01xfbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1hv9uaj</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">42 days later… </t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv9uaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1hv9lpx</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>my sweet piano nails! ₊˚⊹♡🎀</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv9lpx</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1hv92ma</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Refresh ideas please!</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv92ma</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1hv90dl</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>I love when they match</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pypa87imofbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1hv8ppi</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>🤗</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rp4xf68jmfbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1hv8p0j</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Love my new set</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfcrymmemfbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1hv8o9c</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>What should I do with these two nails?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv8o9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1hv88sr</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It’s winter!🥶 </t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctjnyw18jfbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1hv7g86</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>January set</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv7g86</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1hv7g68</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>New Year, New Nails :)</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jk4pbyhdfbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1hv791j</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>i need help finding this shade!</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lj0hk643cfbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1hv6urk</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Pink for Jan 🌸</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv6urk</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1hv5wel</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail art ideas </t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bahcvk5b2fbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1hv5yfl</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Asked my tech for nails inspired by Howl's Moving Castle</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2spw1owp2fbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1hv6j5s</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First ever set with no practice </t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/atb2rl9v6fbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1hv5scw</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this a fake product? </t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv5scw</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1hv4x2k</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">end of Dec going into Jan Set </t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03o6pk96vebe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1hv4pzf</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Rose Gold on point!</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0gsslnqtebe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1hv4n9m</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New year, new set 💅🏽 </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv4n9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1hv4jh4</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>January nails</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pssw9sggsebe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1hv4dy8</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First full acrylic and frenchie set. Feedback appreciated! </t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv4dy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1hv458o</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Black and Grey</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hv458o/black_and_grey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1hv44h5</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Patek Philippe set</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv44h5</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1hv43m2</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Cost of Gel Overlay</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hv43m2/cost_of_gel_overlay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1hv36z8</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>🍒</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukto9gbriebe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1huwi5v</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For business formal and networking wear are almond glazed donut nails good? </t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1huwi5v/for_business_formal_and_networking_wear_are/</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1huz07a</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Are my nails long enough to try shaping them? What shape should I try? What can I do to improve my nails?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1huz07a</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1hv0imo</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Dazzledry?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hv0imo/dazzledry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1hv1a2c</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Why do my nails bend like this?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv1a2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1hv2nm9</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for advice </t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv2nm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1hv2xma</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI Repair Mode question </t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hv2xma/opi_repair_mode_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1hv2ubq</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>New Year's look!</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv2ubq</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1hv2nl3</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Winter Nails 💜🩵🩷</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv2nl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1hv2hux</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>FINALLY getting some promising growth!</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv2hux</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1hv0wsj</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>What my client sent me vs what I made. What do you think?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qco9s9jc1ebe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1hv0jr7</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv0jr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1hv0ihg</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>husband said orange so I came up with tropical orange</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv0ihg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1hv0a0w</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Dark blue and glitter should never be missing ⭐️💙</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlbxnw42wdbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1hv035n</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>c-curve stiletto press-ons!</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv035n</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1hv00g0</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails keep peeling and breaking </t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hv00g0/nails_keep_peeling_and_breaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1huzgtx</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Nails perpetually weak, thin, breaking</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1huzgtx</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1hvmqds</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you decide your next manicure? </t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvmqds/how_do_you_decide_your_next_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1hvmq1n</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t xml:space="preserve">polishes that look like this? </t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvmq1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1hvkxkp</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Swatched and labeled my collection 😍🤩</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avxxzcb9iibe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1hvk2aj</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Peel off base for press ons?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvk2aj/peel_off_base_for_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1hvjxxr</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>OPI Nail Lacquer Never Dries?</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvjxxr/opi_nail_lacquer_never_dries/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1hvjn9s</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4p5ec0k4ibe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1hvjai0</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>F in the chat for my fallen soldier</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvjai0</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1hvj2wv</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>A color to go with the cloudy skies</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvj2wv</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1hvivpa</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Matte matters</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvivpa/matte_matters/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1hvibxb</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>First at home gel mani !</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvibxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1hvi072</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Loving flakies rn!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qudd6ptohbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1hvhdcb</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Bone &amp; Parchment</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvhdcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1hvhazm</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Favorite warm polishes?</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvhazm</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1hvgukz</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>December Manis 🎄🎁</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvgukz</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1hvgj3t</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Storing thermals in the fridge? Does anyone do this?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvgj3t/storing_thermals_in_the_fridge_does_anyone_do_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1hvg6vq</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>How do people usually do the logistics of destashing?</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvg6vq/how_do_people_usually_do_the_logistics_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1hvfzqf</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Looking for color like ILNP Dash of Cocoa without holo</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvfzqf/looking_for_color_like_ilnp_dash_of_cocoa_without/</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1hvfpok</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Alright, y'all inspired me. Starting a My Year in Nails 2025!</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3oh4iwd4hbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1hvfpmx</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Honest and In-Depth Review of OPI’s New Rapid-Dry Polishes</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3rtn56td4hbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1hvfnje</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Still trying to figure out how to add rhinestones without getting glue everywhere</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvfnje</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1hvfjry</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone else get a “craving” to wear a certain color sometimes?? Or am I just weird? </t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hb45kko13hbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1hvf1cn</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Apparently, the Gym has the best lighting</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvf1cn</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1hvel5a</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Newbie needs help!</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvel5a/newbie_needs_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1hvebga</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tengo un problema con mi esmalte de unas </t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvebga/tengo_un_problema_con_mi_esmalte_de_unas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1hve7bt</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Ashes When They Cremate Me 😩🙏🏼 </t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mtp4p1pyrgbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1hvdwjp</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>There’s always that *one thing* that exactly matched your nails. This time around it’s edamameeeee</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0sfrdumpgbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1hvdd9v</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Colors</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvdd9v</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1hvd38d</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Looking for a blue with pink shimmer</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvd38d/looking_for_a_blue_with_pink_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1hvcs7y</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Winter morning vibes</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvcs7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1hvclxv</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For my Orly fans: check your TJ Maxx! </t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ftjyt6bfgbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1hvcjjl</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>I guess I have a fav shade of pink</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvcjjl</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1hvchy3</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>OPI v. Holo Taco husband thinks OPI is best; can y’all help me “sell” him on HT?</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvchy3/opi_v_holo_taco_husband_thinks_opi_is_best_can/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1hvcdvo</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does lurid lacquer ship internationally? </t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l51yor5kdgbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1hvca26</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>she could never disappoint me</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/25pqv84kcgbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1hvbq2f</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>This Lurid polish practically glows!</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6cexoga8gbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1hvbnll</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Best smoothing topper for glitter polish</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvbnll/best_smoothing_topper_for_glitter_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1hvbbbq</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any Canadians know where to get Nailtique? </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvbbbq/any_canadians_know_where_to_get_nailtique/</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1hvb3qn</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Help finding a top coat that doesn’t crack?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvb3qn</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1hvaxdi</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>First time trying a magnetic!</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvaxdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1hvax5s</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Anyone else doing a palate cleanser as their first mani of the year?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvax5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1hvauoo</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>First time trying magnetics🩷💚</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hreoj5mw1gbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1huz3zi</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Anyone wants to order Cirque together in Vienna (for free shipping)?</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1huz3zi/anyone_wants_to_order_cirque_together_in_vienna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1hv3lzn</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>cuticle remover</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hv3lzn/cuticle_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1hv6gkx</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>I’m no nail artist, but I’m really happy with how these colorful plaid jelly nails came out!</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv6gkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1hvaezm</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Sally Hansen Holographic Line??👀</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvaezm</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1hvadqz</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>mooncat's Imperial Stormtrooper</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvadqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1hv9547</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Magnetic Pigment “Disappears”</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hv9547/magnetic_pigment_disappears/</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1hv8v0v</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Everyone wants to be her </t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv8v0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1hv8mxm</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>First Mani of 2025!</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ja7ezk4zlfbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1hv8l2r</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Was hoping for glazed. Not what I got but still a fan</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyap7h8mlfbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1hv7yrb</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Red/purple/blue shimmer polish?</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv7yrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1hv7taz</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Winter weather had me feeling in the mood for red ❄️🍎</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n91hntk7gfbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1hv7ibn</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Pinks for someone who hates pink?</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hv7ibn/pinks_for_someone_who_hates_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1hv7hku</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Loving these celestial blue vibes from DT!</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jqiq8gtdfbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1hv7f47</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails in December! </t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv7f47</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1hv6wkg</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Nail treatments that work under polish</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hv6wkg/nail_treatments_that_work_under_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1hv5ais</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emily de Molly skittle! </t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv5ais</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1hv53wx</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Good drugstore ridge filler and/or blurring base coat?</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hv53wx/good_drugstore_ridge_filler_andor_blurring_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1hv4gvk</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>You already know what it is 🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv4gvk</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1hv4cb7</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>A Galaxy 😍</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv4cb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1hv42fo</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Gengar 💜</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv42fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1hv3hh5</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BKL Daydreams </t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gs064c4wkebe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1hv3anl</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Starting off the year with a flaky bomb ✨</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sotjtqrhjebe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1hv2vzv</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>BKL, I Choose the Bear 🐻</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6ih4z2egebe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1hv2l9a</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Crackle over Magnetic (pics in comments)</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/02v91nb7eebe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1hv1nm9</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>🤩</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ty5z71h57ebe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1hv1hsd</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>So Pretty... So Painful</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/815v5fhv5ebe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1hv1b7m</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Possibility of Snow Calls for Thermal Polish! </t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv1b7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1hv16tx</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Got 20 essie nail polishes for $25 and I'm skittling my way through.</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ka4jfeg3ebe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1hv0vc5</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>🌊🌊The Great Wave🌊🌊</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv0vc5</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1huzt8s</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Tried something new! Its messy, but I'm excited for the potential of the next attempt!!</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1huzt8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1huzqx1</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>First time trying magnetics. Not sure I did it right…</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iy4yj4virdbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1huczwg</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice on nail product gifting!! </t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1huczwg/advice_on_nail_product_gifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1hunvzv</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A question to Nailtechs </t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hunvzv/a_question_to_nailtechs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1hup9qi</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Are nail allergies really as common as they seem???</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hup9qi/are_nail_allergies_really_as_common_as_they_seem/</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1huyjm1</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Help identifying my OPI polishes! 🩵</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1huyjm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1huwjp6</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1huwjp6/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1huw3dq</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>BKL Magnetic question</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1huw3dq/bkl_magnetic_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1huuvxt</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat’s mercury’s tears 💧 </t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nzcb00ia9cbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1hvktdh</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>New year new me</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvktdh</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1hvj5b4</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Starry New Year</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvj5b4</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1hve0f4</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Silver Chrome Nails 💅 </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ee5kb1fqgbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1hvb3op</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Painted this mini Irn Bru can to test myself 😮‍💨 My wrists ARE SHAKING from being so strained 🤣🫶🏼</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bto0rzrr3gbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1hvag9a</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>My favorite DIY holiday nails from this season</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mwmh7kzyfbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1hv9zar</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Reverse painting waterslide decals</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvknu1jjvfbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1hv9x1r</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>my sweet piano tea party nails!⊹♡🎀</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv9x1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1hv62to</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my xmas nails </t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv62to</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1hv414s</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Patek Philippe set</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv414s</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1hv36lk</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>🍒</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpizu0boiebe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1hv2tie</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Winter Nails 💜🩵🩷</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv2tie</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1hv0l2j</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>“Monet”/oil painting style nail</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hv0l2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1hv0320</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>I love pink 🩷</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4my762nfudbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1huujus</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>inspired by “thenailbender” on instagram 🖤</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3voguqjo4cbe1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jan  8 08:10:54 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_12.xlsx
+++ b/data/collected_data/2025_01_12.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C494"/>
+  <dimension ref="A1:C685"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8831,6 +8831,3259 @@
         </is>
       </c>
     </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1hwe2lj</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Blupink ?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7g9iy4zypbe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1hwdxar</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>My crooked little fingers👄💅🏻</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwdxar</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1hwdlhc</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Can't tell if this color is flattering or not ?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwdlhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1hwdf9z</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>any suggestions for the best strengtheners and cuticle oils?</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hwdf9z/any_suggestions_for_the_best_strengtheners_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1hw8rt7</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Does anyone know of a good website that has a variety of press on nails for people with wide nail beds?</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hw8rt7/does_anyone_know_of_a_good_website_that_has_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1hwc5aw</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Gel polish on metal?</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hwc5aw/gel_polish_on_metal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1hwb30q</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help? </t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80t9r55c3pbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1hwc2b2</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Nail Help!</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hwc2b2/nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1hwc3ph</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9au15ibmdpbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1hwboda</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying something new </t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3upi1u0c9pbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1hwbd55</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Lamps..</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hwbd55/lamps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1hwb1e6</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>i want to start doing press on sets, are soft gel tips okay for that?</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hwb1e6/i_want_to_start_doing_press_on_sets_are_soft_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1hwao0u</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The 1st tone of 2025.. </t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1m4xdivbzobe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1hwaniv</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nude XL almond set I did on myself tonight! </t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l096apz6zobe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1hwac3r</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>January set</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwac3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1hw9vow</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>HATE pushing back my cuticles, any alternatives?</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hw9vow/hate_pushing_back_my_cuticles_any_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1hw9upy</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails I had for the holidays </t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nip281aprobe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1hw9qt4</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>New Nails For January</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4k7vd7qqobe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1hw9c5w</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>how are these nails?</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84wjvb1ymobe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1hw8ina</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>At Home Setup Tips</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hw8ina/at_home_setup_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1hw8goh</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it possible to keep water out of press-ons if you're always in it? </t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hw8goh/is_it_possible_to_keep_water_out_of_pressons_if/</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1hw7x3a</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Fav new nail color</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6yoreglaobe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1hw7u11</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>SMILE :)</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw7u11</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1hw7thb</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Do these look like press-ons?</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw7thb</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1hw7rad</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I am obsessed with vampire-y looking nails </t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9l3h05u69obe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1hw7qd7</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Teal &amp; White with chrome 🩵🤍</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw7qd7</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1hw6lml</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Pastel nail design</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ec44g0z7znbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1hw5zy1</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing extensions and nail art. Any tips? </t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw5zy1</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1hw4n5y</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Please Help - a girl who loves her nails</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/leux9p9gjnbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1hw5xyg</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting duck nails </t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2buspu6xtnbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1hw5c9d</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying gel dip at home! </t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw5c9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1hw54ys</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>So cute and girly🩷✨</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bhft9fbnnbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1hw52w0</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Perfect </t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/loldocfumnbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1hw4k6k</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Do I have long or short nail beds?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzvcj89tinbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1hw3yu2</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The difference between my sister and myself </t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw3yu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1hw3p8q</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Favorite sets I did in 2024</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw3p8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1hw3lsy</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Does cateye require UV ligths</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hw3lsy/does_cateye_require_uv_ligths/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1hw3emm</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Missing my favorite summer nails 🍒</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cig174mx9nbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1hw3d8a</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Took a break from work to admire these beauties</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcf5dppq9nbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1hw2npc</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>How did they turn out for me?</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw2npc</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1hw1wm6</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thermal nail polish </t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw1wm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1hw1vap</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>May your new year be as bright as my nails 🎊</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltoozahlymbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1hw1sq7</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Fresh January mani</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnsxbxn2ymbe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1hw0syh</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Which nail shape on me?</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw0syh</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1hw0pkg</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone recognize the brand from the swatch? It’s a gel that came with a magnet at a local salon </t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5y0ccifzpmbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1hw0dc2</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>my long natural nails currently ✨</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw0dc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1hw09h9</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>New nails &amp; they glow in the dark 🙈😇</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw09h9</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1hw05hg</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you put on first </t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okwrqb1xlmbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1hvzz3v</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is hard gel just not for me? </t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvzz3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1hvz35o</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Who is to Blame?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvz35o</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1hvz2wg</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Who is to Blame?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvz2wg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1hvyxu2</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>A little bling for dreary winter days.</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvyxu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1hvyxa8</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first gem set! </t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvyxa8</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1hvyr5m</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Back to basics </t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tu9whvcobmbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1hvyl2h</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Nail shape for Wedding?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xyxuw5heambe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1hvyi3f</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Getting better</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvyi3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1hvy0yx</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please tell me they're nice before I start crying </t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvy0yx</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1hvxtwt</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>i got some nail stickers for christmas and did my first set with them ♡</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dprvspms4mbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1hvwrbg</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Did my own nails!</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvwrbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1hvwbid</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>First time 3D nails</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvwbid</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1hvwbb2</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>how to keep nails healthy while having an intense job?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hvwbb2/how_to_keep_nails_healthy_while_having_an_intense/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1hvwazo</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Pinterest Ad</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qxd4czrtlbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1hvuvl8</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tired of my natural coffin shape - I’ll try almond before cutting them off completely </t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvuvl8</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1hvva1a</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Black and rose gold</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvva1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1hvv7u9</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This set on my tattoo artist is just.... Perfect! </t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2eumo7nllbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1hvussm</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new years eve/ year of the snake inspired :) ✨ 🐍 </t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/me0hv27iilbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1hvu443</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>A Huge Thank You to All of You.</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hvu443/a_huge_thank_you_to_all_of_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1hvpo9g</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>First time press ons</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hvpo9g/first_time_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1hvre9l</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>How do I get nail glue off Matt nails</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hvre9l/how_do_i_get_nail_glue_off_matt_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1hvumhj</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>A fun pop of color and bling! ✨</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nrwenz07hlbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1hvuk6j</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Rainbow Frenchies 🌈</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2rgurmpglbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1hvuf6f</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Now That The Christmas Period Is Over, I Can Go Back To My Gothy Nails </t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvuf6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1hvueh1</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>First ever fully gel set— New Years cat eye french with real encapsulated rose quartz!</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvueh1</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1hvua2t</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Classy Vacay Nails</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hvua2t/classy_vacay_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1hvu4wq</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Dark Floral</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iimpnn1edlbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1hvtuti</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Im in love with my new set :3</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1ud67u3blbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1hvtiyr</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Night sky set 🌟 </t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmb1uw8f8lbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1hvsv2u</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>My Brown nails</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j522884x2lbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1hvsqpk</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Can’t remove acrylics! Help!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3qzp27w1lbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1hvskwy</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Gotta stay ready 💅🫣</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DEhwy_cpwlO/?igsh=MTl0MnlocmZjcnNrZA==</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1hvsb0l</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do we think </t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvsb0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1hvrn90</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Obsessed with this color</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87buire6skbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1hvrmwa</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>I got an awesome manicure today</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66mppsfxrkbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1hvrh5a</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>What is the difference here?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7oq7u5lqkbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1hvqzqf</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>My amethyst nails. 😍</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvqzqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1hvqzd0</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Tried some cheap ABS Press on Nails for the first time</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvqzd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1hvqj0x</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>new🤠🤠🤠</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fqu3sz6hkbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1hvpvyj</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Tips for tinkering with long nails?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hvpvyj/tips_for_tinkering_with_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1hvpbzn</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>New year nails</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/102txsuw3kbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1hvofq2</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Invader Zim Nails!</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j831iazfsjbe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1hvof4z</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Long nails vs Gaming</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvof4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1hvnvtt</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time doing gel nails:3 </t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwoqp43skjbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1hvnvgs</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>A classy set always 🤍💕</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zsqzubnkjbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1hvnkzh</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Is this one of those top coats that will harm me long-term if I’m not careful around my cuticles?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvnkzh</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1hvndh0</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Christmas it's over but I still have this 😳</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3jnv0nsdjbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1hwdywu</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Reviews on Holo Taco at Ulta?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hwdywu/reviews_on_holo_taco_at_ulta/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1hwdn1t</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers - My Pet What?! ft my own sweet pet assisting with posing my fingers</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwdn1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1hwd5i0</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made a watermelon! Also these colors are so juicy I want to eat them. </t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwd5i0</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1hway1a</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Accidental match</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hway1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1hwaa38</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Blue Pick Me Up</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0a58wvxovobe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1hw9zkf</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Magnetic nail polish </t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hk99liwysobe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1hw9xf8</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>🐆❄️Snow Leopard❄️🐆</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw9xf8</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1hw9dpi</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Nail shades recs for wedding</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9noxkpncnobe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1hw987q</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Mooncat Millennia is really magical ✨</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw987q</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1hw973s</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polished for Days or Emily de Molly? </t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw973s</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1hw90q2</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>my new favorite combo ❤️</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw90q2</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1hw8cwp</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Multichrome(?) skittle </t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0z6iqqcz8obe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1hw8093</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ”Reverse” velvet! </t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw8093</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1hw7zfw</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Scum and Villainy: worth the hassle? </t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x5rumkr4bobe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1hw7z18</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>✨ first attempt at galaxy magnetic nails! 💫
+🌌
+1 x ASP longwear basecoat
+1x ILNP ink
+2x ILNP deep space
+stars from Over The Top Nails
+1x mooncat speed demon top coat</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw7z18</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1hw79db</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>blue birddddd 🐦</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uin0zskv4obe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1hw73px</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Favorite polish name</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1bgfr9ri3obe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1hw6p6e</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>my October HHC order finally made it to me in Canada!!</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw6p6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1hw6f1x</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Cheap chrome powder over translucent brown jelly. The translucent brown makes that chrome GLOW. Winning combo for me.</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aaeo4gunxnbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1hw691k</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>💜🔮✨</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yr7abakbwnbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1hw67vb</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>An Oldie but a Goodie</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ct1i3uc0wnbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1hw663v</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Guess the price</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw663v</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1hw5x0r</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Looking for more glitters with jelly base</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hw5x0r/looking_for_more_glitters_with_jelly_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1hw5i56</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Nail tech buffed through my nail…</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8oi0kim9qnbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1hw5cty</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>LynB Designs Snow Joking Matter</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw5cty</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1hw4nqq</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>So…what do you do for fun after work? 😂💁🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw4nqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1hw4l94</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Shout out to this drug store polish as a potential blurring base coat</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kapshuh1jnbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1hw43cj</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>More orchid, more glow!</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uejfxns0fnbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1hw35q4</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Finally getting around to keeping my nails painted regularly</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10gzhqt78nbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1hw32ke</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Please help me clean up the cuticle area better!</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mfxr7ddj7nbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1hvzed7</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Few weeks of mani's and </t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvzed7</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1hw2u2x</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Mooncat Frosty Blues 🩵❄️🧊</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw2u2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1hw2sni</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Starting the new year off rosy 🌹</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdsgosrc5nbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1hw2fk2</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t xml:space="preserve">missing package finally arrived! </t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mtc47x0q2nbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1hw2dkv</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Patty Lopes - not like photo</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3tdaju9b2nbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1hw20iv</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help ID this glimmering peach color </t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hw20iv/help_id_this_glimmering_peach_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1hw1wmv</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>May your new year be as bright as my nails 🎊</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyfllwmuymbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1hw19fu</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Shifty Goodness</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw19fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1hw0wp6</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Something Green </t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw0wp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1hw0jwk</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Magma Reaper Across the Multiverse</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u2ydgnfmombe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1hw0211</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Manicurist? Shine</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hw0211/manicurist_shine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1hvzrci</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Alibi 🦋💙 Also gyms have great lighting for taking pictures of your nails ✨</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvzrci</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1hvz7rl</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>How can I get this green nail polish out from my nail bed ?</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tllv7640fmbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1hvz68m</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Loving this cheap blue holo!</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gd78zizoembe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1hvyr8t</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Seche Vite surprise effect</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9s7y9d3pbmbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1hvyjuf</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Topcoat Recommendations </t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvyjuf/topcoat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1hvyhw8</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Starry midnight sky...</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvyhw8</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1hvy3q6</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>in love not given lightly ✨</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvy3q6</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1hvxywm</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Weekly Mani</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7zs4q7u5mbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1hvxyuz</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Y’all are such a bad influence 😂</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uk4e0avt5mbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1hvxual</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Oh she’s a shapeshifter💕</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvxual</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1hvxp2w</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Shameless Self Promotion 😇</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvxp2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1hvxl1t</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>:)</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvxl1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1hvxemf</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DRK Nails (PPU Dec '24) Happy 2025 😍 </t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nw7gsutp1mbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1hvxe5m</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>How do I stop my nails from looking like this after I remove laquer?</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvxe5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1hvx22d</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mixed up nail curvature?? </t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvx22d/mixed_up_nail_curvature/</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1hvwowq</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Got my nails done at the salon for the first time I love how shiny they are but she didn’t get very close to the edges is this normal? Also how can I fix my pointer nail</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvwowq</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1hvwi2g</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>You were all right, Deep Space is amazing and I needed it</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvwi2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1hvw8ib</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love seeing your nail art so here's mine (not very good but not SO bad) </t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/isdfge49tlbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1hvw069</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bestie pup made a good background for the Polish. Almost one month of no nail biting! </t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvw069</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1hvvzjq</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Okay, this is clearly sorcery~</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z14uqjdhrlbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1hvvy0c</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>They're short also help with jelly</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvvy0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1hvvnzm</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quiet </t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ef2ik542plbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1hvvmwa</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Jade nails</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5asa9gstolbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1hvvfcu</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>new year, new nails ♥️</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvvfcu</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1hvvf08</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>A classic favorite that back in the day you used to be able to get for $0.99 on sale at Walgreens….Sinful Colors Endless Blue 💙</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpmmdwz5nlbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1hvveaf</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Free Gift In Cupcake Polish Order?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvveaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1hvv0c1</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Opal shorties</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvv0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1hvubmx</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Thoughts on gold/brown with my skin tone? ILNP Fawn in the sun 💛✨</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvubmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1hvu4oz</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fav pedicure colors </t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvu4oz/fav_pedicure_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1hvtx94</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Folie à Deux </t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvtx94</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1hvszbc</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>How long for holo taco to ship?</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvszbc/how_long_for_holo_taco_to_ship/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1hvpixn</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel IQ - should I continue or switch? </t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvpixn/gel_iq_should_i_continue_or_switch/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1hvs470</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polish longevity reviews </t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvs470</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1hvrtzn</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Winter soft girl, with a no-clean-up marbling technique!</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcr5jegwtkbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1hvrqrd</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gay af skittles </t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvrqrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1hvrf0f</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Do you ever nearly finish a mani, decide you hate it, and remove it immediately? 😅</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvrf0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1hvraw2</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A story in 3 parts </t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvraw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1hvg1su</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>What to do with my gel products???</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvg1su/what_to_do_with_my_gel_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1hvosyr</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>What colors are we feeling for Jan &amp; Feb</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvosyr/what_colors_are_we_feeling_for_jan_feb/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1hvo6vs</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opinions on Revlon Clear? It's my go-too top coat, and I wonder why it isn't more popular. Others i've tried includes Gel Setter, Gel Couture, and Insta-dry. </t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hvo6vs/opinions_on_revlon_clear_its_my_gotoo_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1hwbryc</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o7mmungcapbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1hwal01</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🌷Try out some cuties with tulip vibes! </t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1wfy3driyobe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1hw8apm</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Nail</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrvgjkywdobe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1hw7l7q</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>arcane hextech nails ✨</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw7l7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1hw7ed8</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>How much would nails like this cost in Canada?</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irzovap16obe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1hw6r57</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>What nails would look good for this Valentine's Day?👋🏻❤️</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hw6r57/what_nails_would_look_good_for_this_valentines_day/</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1hw6719</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time working with nail molds! 🩷 Coquette nails </t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw6719</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1hw6202</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first proper hand painted set I did as part of my art college work! </t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5y407nntunbe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1hw5ira</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>cutesy little apple nails ! practicing my nail art lol.</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gw9pvmsbqnbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1hw40ks</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tips in how to improve </t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hw40ks</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1hw2umt</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>My Capricorn glam birthday nails</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sui7q5tv5nbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1hvxlqj</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Coraline Nails 🕸️</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvxlqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1hvwlvc</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Ice Queen Set</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p5hd2euyvlbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1hvu9sl</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stars nail art </t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4o0rfxvgelbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1hvppuv</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>some metallic nails i made</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hvppuv</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jan  9 08:10:51 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_12.xlsx
+++ b/data/collected_data/2025_01_12.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C685"/>
+  <dimension ref="A1:C859"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12084,6 +12084,2965 @@
         </is>
       </c>
     </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1hx7gtu</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Pink and orange ombré chrome 💕🧡</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5ed9kjd6xbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1hx72zp</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 minute manicure </t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ya0s33de1xbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1hx6saw</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Soft-Gel Nails</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hx6saw/softgel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1hx6l9w</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>nail shape</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx6l9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1hx6hzu</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chocolate bear </t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1txrb1p6uwbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1hx42jf</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>What are some good starter product recommendations?</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hx42jf/what_are_some_good_starter_product_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1hx5ldq</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>What shape are my nails?</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx5ldq</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1hx5iw3</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx5iw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1hx5ec7</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Everytime I think "this'll be the set!" it ends up being dookey</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx5ec7</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1hx5d34</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>What the best polishes for press ons</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hx5d34/what_the_best_polishes_for_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1hx54c0</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>New year, new nails!</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dfoqttbfwbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1hx4wfz</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter nails love </t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqb09ig0dwbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1hx4juj</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>feel like i went to war to get my acrylics off</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/un7fmg2i9wbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1hx4cop</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Anyone’s fingertips get cold with gel mani?</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hx4cop/anyones_fingertips_get_cold_with_gel_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1hx3lay</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t xml:space="preserve">a nice little neutral reset </t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx3lay</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1hx3fnd</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Do my natural nails look compromised?</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx3fnd</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1hx2sx0</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Ditto nail art by @uranakadesu in Osaka</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx2sx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1hx1vq1</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Fresh set</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gegns1jumvbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1hx1rhm</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>brown seasonal nails!</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6lvtumvlvbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1hx16um</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>What’s everyone doing for Valentine’s Day nails??</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hx16um/whats_everyone_doing_for_valentines_day_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1hx10io</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help identifying maker/model? </t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx10io</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1hx0kpu</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m about to start getting my nails done for the first time ever - Should I do gel x, acrylics, dip with tips, or grow out my natural nails somehow? Photos attached </t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx0kpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1hx0gqa</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Got Gels!!! Feel so pretty!</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i21skgjlavbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1hwzvlo</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>flow 2000</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tib2pkah5vbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1hwzure</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>I love my delicate nails with butterflies 🦋💅</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4k9r0s95vbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1hwzlit</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first set of 2025 </t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69ti39s13vbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1hwyt9i</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Just did these magical fairy princess nails</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwyt9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1hwypsr</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glass nails: How to get the look </t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/csdvijohwube1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1hwy4yi</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>icicle nails for january🧊</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2ait4fbsube1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1hwy2ve</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Winters January Vibes 🩵🩶🤍🖤</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r9ysd7jvrube1</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1hwvyyu</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to find polish colors that look the best on you? </t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hwvyyu/how_to_find_polish_colors_that_look_the_best_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1hwwsbp</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Apres Nail Tips and Sizing</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hwwsbp/apres_nail_tips_and_sizing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1hwsg00</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question about nail health </t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwsg00</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1hwwana</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t xml:space="preserve">looking for advice about nail extension options </t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwwana</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1hww8k0</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Molten gold to kick of 2025 💅🏻</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3cgrh64eube1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1hww65d</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Short nail love</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hww65d</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1hww5ag</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>My gal is one of the best 🥹🫶</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hww5ag</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1hww1he</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Classic Gel-X French</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hww1he</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1hwvui4</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Hi! I'm debating btartboxnails but am wondering, do I have to use gel polish with them?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hwvui4/hi_im_debating_btartboxnails_but_am_wondering_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1hwvsis</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Non-exclusive nail gang </t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zh7lu0sxaube1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1hwvsdh</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Is there any saving this nail, or should I finally give up?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwvsdh</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1hwvlpn</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Unhappy with 30th birthday nails :( please help</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwvlpn</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1hwvfor</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>chrome powder fell</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hwvfor/chrome_powder_fell/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1hwvbyv</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting a pedicure. Are arcrylic nails supposed to be thick like this? </t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwvbyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1hwva35</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Halfway There!</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwva35</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1hwun5g</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Press Ons</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwun5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1hwuglc</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Current mani</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/goirh36z0ube1</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1hwufkd</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Smudged essie gel couture </t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nswgadsr0ube1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1hwu2n6</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Dreaming of Ghibli ☁️ ✨️</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwu2n6</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1hwtwma</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple sparkles </t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3vcfgauwtbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1hwsrvn</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Got my first set in 3 years!</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwsrvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1hwtgql</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>New year, new nails 🖤</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/by8tseeittbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1hws7dv</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas gift </t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hws7dv/christmas_gift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1hws5cz</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye 🐱 </t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2grag5rjtbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1hws47t</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Flames 🔥</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/meqt6y8ijtbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1hws2ox</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red </t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x49gh6y6jtbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1hwrtz7</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>January nails</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o300atlhhtbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1hwrnbh</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Bambi nails 🦌 inspo from @kkstricklnd on Pinterest</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwrnbh</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1hwpptm</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cracked nail </t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4rbvd0d32tbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1hwqmie</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Why do my nails grow transparent in random spots?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwqmie</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1hwrdwr</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Nail growth journey, doing my nails at home 🙏</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwrdwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1hwqgfr</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I need tips </t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hwqgfr/i_need_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1hwptye</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tragedy to Triumph </t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwptye</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1hwpbyj</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>The glow nails of my dreams</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwpbyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1hwqvam</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inspo from this subreddit. These turned out so cute! </t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0po9tkfatbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1hwr9yq</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>OPI Pink in Bio 💕</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwr9yq</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1hwquaq</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hands </t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iogvfc58atbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1hwqtv6</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Ladies, would you date a guy who wears polish?</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hwqtv6/ladies_would_you_date_a_guy_who_wears_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1hwqp2c</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Nails I did on myself and my sister in 2024</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwqp2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1hwqlm2</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>First time getting acrylic nails, is the inside supposed to look like this?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwqlm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1hwqiy5</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cringe personalised AI video from Sassy Saint </t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eacfdrru7tbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1hwpj5n</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>[HIRING] Nail Technicians – Watervliet Nail Expo</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hwpj5n/hiring_nail_technicians_watervliet_nail_expo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1hwphbc</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sweater weather! </t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwphbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1hwpeio</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sorry I like this pic better </t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwysit5szsbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1hwovmq</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>First set of ‘25! Cool toned pink + mermaid 🧜🏽‍♀️</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xu00syb1wsbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1hwosac</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>2024 nail recap ⋆˙✮</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwosac</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1hwomap</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 week of growth. </t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwomap</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1hwoin7</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>My first test set!</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzs0wq6jtsbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1hwo9zh</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Junk set💖</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwo9zh</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1hwnpf4</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I hit window too hard not knowing my finger is in between and slammed is hard and now i have this. One of the most horrible experiences </t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60qcseclnsbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1hwnfuu</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time in forever! ✨</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3ljb4wplsbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1hwlf3l</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another year, another fresh set of nail stickers </t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwuqrknd5sbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1hwm63l</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>how do i treat this! :(</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/limanawobsbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1hwn0bt</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to make non gel nails polish last longer </t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hwn0bt/how_to_make_non_gel_nails_polish_last_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1hwmm4x</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is so prettyyy </t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwmm4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1hwltcg</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Cuticle removal?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwltcg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1hwlcb8</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Shaping advice</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwlcb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1hwkq3q</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>(Poly)gel nails another layer after topcoat?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hwkq3q/polygel_nails_another_layer_after_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1hwkdpd</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I made these and i’m so proud! </t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwkdpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1hwjzbm</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Help… should I go back ?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwjzbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1hwjthh</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>My new manicure - I think red is the color of passion</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q60fhpgvqrbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1hwhi3y</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Went over the cuticle area while buffing (acetone soaked) hardgel off with a coarse file, and it takes forever to heal. Send hugs.</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1w5f4ipj3rbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1hwf4c5</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Care Advice Needed ! </t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwf4c5</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1hwfbtm</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>I hate my nail shape!</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmspzllqdqbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1hwfznh</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>just here to show off</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwfznh</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1hwhoe5</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t xml:space="preserve">essie - hi maintenance </t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hwhoe5/essie_hi_maintenance/</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1hwj9bn</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So indecisive </t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjohbd4ulrbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1hwiexc</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Micro french 💅</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwiexc</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1hwi5l9</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think of these little flowers? </t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2kfqt5narbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1hwhw4g</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivbe7glt7rbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1hx83t5</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Photos don’t do it justice! My first ILNP</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tisai95texbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1hx7tu1</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Carly and my nails.</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx7tu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1hx77cz</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t xml:space="preserve">advice for a beginner trying magnetic polish </t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hx77cz/advice_for_a_beginner_trying_magnetic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1hx5b66</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Beetles is pushing regular lacquer, perhaps in an effort to get back all the customers they gave gel allergies 🙃</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx5b66</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1hx52od</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>I can almost hear the John Williams score</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hqq09inuewbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1hx4ulb</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Found my original nail art stash from 10-11 years ago. Anyone remember these?</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/821b26ekcwbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1hx4qx1</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP La Catedral </t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx4qx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1hx4lol</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>First skittle!</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v9gg9sc0awbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1hx4hn7</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Fierce Mojo vs. Fool’s Paradise???</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx4hn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1hx4a8z</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Wore press-ons and this is how the base of my nails. Anyone else see this before?</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5m4upcfu6wbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1hx47pg</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Anti Allergy Laquer</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hx47pg/anti_allergy_laquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1hx3uka</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink base color suggestions? </t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1md5uir73wbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1hx1rq8</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Thermo nuclear from Clionadh</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3imv0ajxlvbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1hx12pv</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Any ideas how to do this? (with regular polish)</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ca121gd0gvbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1hx0haa</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Keeping it simple</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx0haa</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1hx0cu0</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Dad's solution to a horseshoe magnet</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hx0cu0/dads_solution_to_a_horseshoe_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1hx0bc8</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Putting my magnets back to work! Circles or velvet?</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5fswtoo49vbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1hx06w2</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Current state of mixed bottle</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2bob8098vbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1hwzzu0</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Zodiac Collab-Labradorite</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwzzu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1hwzbi4</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>A England's She Walks In Beauty. I wish the camera could capture how beautiful this pinkish goldish sparkle is irl</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/42aaec0c0vbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1hwz56t</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Aura nails are harder than they look</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwz56t</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1hwz04z</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Love glossy top coats but matte just hits different. Also first polish of the year</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwz04z</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1hwyjkk</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>How do you pick which polishes to use next when trying to get through untrieds?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5eakxy7vube1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1hwy830</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>What nail shape would suit me?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwy830</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1hwxats</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Am I everything you fear?</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwxats</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1hwwn19</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>How do I fix this at home??😭</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwwn19</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1hwwgr0</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Easy winter manicure! </t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwwgr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1hwvfrb</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Two favorites lately </t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwvfrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1hwv7b0</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Zoya’s annual sale is live: 10 for $25 until 1/13</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://zoya.artofbeauty.com/content/category/New-Year-New-Hue-2025.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1hwunuq</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>It's too much fun watching the colour shift</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwunuq</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1hwulnh</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural look </t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwulnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1hwul8p</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Similar gel polish recommendations like Kiss imPress Flare color</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7u0mpdw1ube1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1hwul72</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Sweater Weather</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwul72</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1hwu4bo</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Did neon tips and hearts🥹</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwu4bo</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1hwtnah</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>winter palate cleanser ✨</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwtnah</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1hwtk98</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Mildly sparkly happy nails to help with January blues</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwtk98</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1hwtesm</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>This ILNP skittle scratches my brain in all the right ways! Featuring: Arcade Collection</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwtesm</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1hwt7fd</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>ISO Cobalt blue linear polish that matches Holo Taco Midnight Spark in tone?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hwt7fd/iso_cobalt_blue_linear_polish_that_matches_holo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1hws28r</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Call for purple nail polish lovers!  Show me your favorite shade!  Influence or de-influence me: Do I need another purple?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5b2xr9e3jtbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1hwr399</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>BKL The Dark Urge is my new favorite thermal 🖤</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwr399</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1hwqx90</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>In search of a duochrome pink/green iridescent topper</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hwqx90/in_search_of_a_duochrome_pinkgreen_iridescent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1hwpv1b</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>When you hit that good lighting 🤌</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwpv1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1hwpqrg</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Lacquer match for this gel color</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0pk46x92tbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1hwp7jc</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>have you ever wanted to swim in a polish?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4ctq9adysbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1hwoe2l</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>How to spot over filing?</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hwoe2l/how_to_spot_over_filing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1hwnucf</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bees Knees Lacquer January launch </t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hwnucf/bees_knees_lacquer_january_launch/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1hwnqxv</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Holy smokes! 😍</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwnqxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1hwmst3</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>ILNP Ava</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwmst3</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1hwmqrw</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favorite polishes for warm  undertones? </t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qh9d62kagsbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1hwm1f3</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Emily de Molly's A Spot In The Woods</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwm1f3</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1hwlxiq</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>✨️🌈Rainbow Armor🌈✨️</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwlxiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1hwln1l</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Blossom - Polished for days</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwln1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1hwlmdx</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Very demure, very mindful 🤍</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1vojhk647sbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1hwlimk</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>What's your opinion: Should nail polish match your outfit/jewelry?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwlimk</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1hwlhwt</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>first set of 2025 ⭐️</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1vaup316sbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1hwkvl5</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Hygge is happening</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwkvl5</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1hwkh33</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Nails inc Got me Glowing - First 2025 mani</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwkh33</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1hwk20f</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone try the brand SSONE? </t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hwk20f/anyone_try_the_brand_ssone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1hwhte5</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top and base </t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hwhte5/top_and_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1hwg3xq</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>ILNP - Rosalie</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwg3xq</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1hx5308</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Mermaid nails, I made these acrylic nails for my birthday (I couldn't take a picture of both hands, sorry)</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uu5tdaofewbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1hx3ky7</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Golden cat-eye star-moon
+It’s perfect for the New Year, but it took me four or five hours</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rc2co93i0wbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1hx374c</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3D clouds and marbled nails </t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx374c</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1hx2nct</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04m28lf3tvbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1hx2j7o</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>New to nail art. How could I get more aesthetically pleasing sets?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx2j7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1hwywaw</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>barbie princess vibes</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwywaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1hwymv1</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Rococo Angels &amp; gold 🪽 👼🪞</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwymv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1hwy0dj</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>added a pearl powder to these, think they were better without 🤔</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwy0dj</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1hws4yu</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Flames 🔥</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqk0ujznjtbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1hwllmq</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>G59 Inspired Nails 🗡️</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwllmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1hwl7fq</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>4th set I've ever made. Honest opinions and suggestions for improvement pls🙏🏻</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hwl7fq</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1hwj8o3</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Looking to learn how to paint press ons on a budget, any tips?</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ln8t9lnlrbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1hwih5k</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Beauty nails ✨</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tj2d7qp2erbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1hwfkhs</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>My nail (gel) polish collection. Which one is your favourite?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9rspfyzqgqbe1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jan 10 08:10:55 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_12.xlsx
+++ b/data/collected_data/2025_01_12.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C859"/>
+  <dimension ref="A1:C1059"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15043,6 +15043,3406 @@
         </is>
       </c>
     </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1hxz88d</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What kinda nails would suit me? Almond or square? </t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpx2j20qd4ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1hxz7tg</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Getting better and better I think!</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c32uag5ld4ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1hxz3kx</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Year of the snek 🐍</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bb8aijbzb4ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1hxyfnq</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>From very strong to brittle &amp; splitting. Help!</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxyfnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1hxyo1b</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Proud of this set I made tonight 🥳</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxyo1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1hxx9e9</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Chrome nails for Coldplay ✨</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxx9e9</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1hxvzrm</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Did my own acrylic and played around with some cats eye polish. I don't hate it! ☺️</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9rx8rqmc3ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1hxvute</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>My first time with stones😍</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6j8osrq6b3ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1hxvu4e</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>French Cat Eye</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vwgm243za3ce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1hxuikd</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Help! Newbie</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vr08na5ey2ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1hxvl8n</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>how to tighten the c-curve?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxvl8n/how_to_tighten_the_ccurve/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1hxvinr</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Color match?</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hemfwebp73ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1hxvd03</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>First time trying a nail design, recently broke a nail and needed to trim them all down RIP</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://imgur.com/WmsZWEd</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1hxv6uz</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some of my diy nails through out the year 💅 </t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxv6uz</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1hxuoc0</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>First Time Nails</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4uahmlvz2ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1hxuiid</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Is this shape as bad as I think it is? I hate it.</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxuiid</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1hxsfjo</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Spiraling out</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxsfjo/spiraling_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1hxtrzd</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Took a chance on a new color and I LOVE it! Yipee!</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9lu9peskr2ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1hxtqwc</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Help! What different gels mean</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxtqwc/help_what_different_gels_mean/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1hxtf03</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel overlay on natural nails </t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxtf03</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1hxteaz</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>So sparkly, I love them ✨🫶🏻</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1m0bwah5o2ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1hxtbwk</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural Nails </t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/heyvfb4kn2ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1hxt6u3</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>what are some of the better gel polish?</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxt6u3/what_are_some_of_the_better_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1hxscc1</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Painting Ellen from Nosferatu for a Nail Set 💞🫶🏼</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5s0nuvie2ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1hxsajx</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t xml:space="preserve">did nail art on my mom </t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxsajx</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1hxs7fy</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Almond shape? It was recommended that I try an almond shape to elongate my nails, any tips or do they look okay? </t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxs7fy</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1hxs114</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>my forever favorite color 💜</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxs114</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1hxrr36</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>What do you think about these nails?✨</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxrr36</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1hxrqm6</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>my nails for today🥰</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atostcl792ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1hxrfp8</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail polish recommendations </t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxrfp8/nail_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1hxr952</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Opal and gold</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxr952</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1hxqxuh</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Tips for very thick, scraggly, dry skin around nails from picking?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxqxuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1hxqxvv</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Am I wrong for wanting to go back and have them fixed?</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxqxvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1hxp98s</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>i’m a 17 year old nail tech, all freehand! pt. 3</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxp98s</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1hxpn38</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Update: Manager did my nails </t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxpn38</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1hxq7sy</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Gel manicures: salon removal and regular appointments</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxq7sy/gel_manicures_salon_removal_and_regular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1hxpdyf</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Tiffany Blue for Jan 😍😍</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53sjza41q1ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1hxp31j</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>How to ask nail tech to cap my nails?</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxp31j/how_to_ask_nail_tech_to_cap_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1hxp2pr</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Are there clear press ons that don’t need gel or acrylic?</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxp2pr/are_there_clear_press_ons_that_dont_need_gel_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1hxod8x</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Allergy?</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxod8x/allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1hxooiz</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>something very natural</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21rm3v9gk1ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1hxoedc</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>First blue set of 2025</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxoedc</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1hxoc9p</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>throwin it back this thurs</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxoc9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1hxoaq8</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Before/after</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4ipg8lhh1ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1hxo25q</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t xml:space="preserve">can you use any kind of magnet for the magnetic glitter gels? </t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxo25q/can_you_use_any_kind_of_magnet_for_the_magnetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1hxnvrn</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A moment for the black cat eye🐈‍⬛ </t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxnvrn</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1hxmeib</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>New nails for the new year!</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpb9126y21ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1hxnm4o</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>whats the best nails shape and length for me?</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxnm4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1hxnbub</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t xml:space="preserve">On the verge of giving up </t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yig3zqbz91ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1hxn9ho</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Pink glitter is always my favorite 🩷</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxn9ho</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1hxn7vz</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Have a hate/love relationship with doing my own nails. But these turned out good i think! </t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1so4fp491ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1hxn562</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>I'm a "more is more" girlie</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxn562</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1hxmxa5</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Batural nails are so weak! Help</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f884nv8w61ce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1hxmb3u</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>My nails are Barbie core and ✨kinda savage✨</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxmb3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1hxmx33</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>As a lifelong nail biter, it feels good to FINALLY have nails! They aren’t perfect, but they’re so much better than they once were :)</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxmx33</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1hxmrh4</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>abstract splatter nails</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxmrh4</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1hxmf6f</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>what type of nail shape would look good with my chubby fingers?</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxmf6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1hxmbj3</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Gel x nail price</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxmbj3/gel_x_nail_price/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1hxm9ts</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>New nail tech 🩷</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmt7he5x11ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1hxm7cm</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>💜💙 I picked up ILNP Birefringence (H) on BF and it reminded me of a polish in my collection with similar blue-purple vibes, Painted Polish Rainbow Fish Wishes. I thought they'd make a cute funky winter mani.</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxm7cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1hxl3xp</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>gel allergy?</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbmw4mc8t0ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1hxldoa</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First manicure in over 5 years! </t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uujvipr8v0ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1hxl81c</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which style fits my hand better? </t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxl81c</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1hxkv9d</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails! 😍 💅🏻 </t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q1xln52fr0ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1hxksf1</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>weird hangnails on my eponychium / nail bed?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxksf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1hxkdab</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>In love with the tortoise shell 😍</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxkdab</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1hxk8id</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Gel Nails with extensions</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k0j2ydtom0ce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1hxk18g</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>2024 in nails - my fav sets</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxk18g</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1hxjtsx</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried cat eye for the 1st time </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxjtsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1hxjkn3</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Irn Bru Nail Set 🧡 For Fun &amp; Giggles </t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6502wferh0ce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1hxjk9j</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>early valentine’s day nails🖤🤍</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6v001l3ph0ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1hxjjph</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Birthday set on myself 🎈</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxjjph</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1hxjb5h</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Would have been so cute but still loving it </t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxjb5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1hxj2qh</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Birthday/ New year's Nails 🎊</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxj2qh</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1hxj01k</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Here are my fully natural nails, what do you all think?</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxj01k</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1hximqb</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>69😏</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hximqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1hxii6p</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>🙏🏽</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afrmykcs90ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1hxi9op</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Safer alternative to gel manicure</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxi9op/safer_alternative_to_gel_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1hxi1k6</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Q for those who have long nails, do you have wrist or hand pain?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxi1k6/q_for_those_who_have_long_nails_do_you_have_wrist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1hxibd1</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>first time at nail salon</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxibd1/first_time_at_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1hxi1tr</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>One of my nails cracked down the middle how do I fix this?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxi1tr</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1hxgymd</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Ghibli inspired soot spirit nails!</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxgymd</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1hxh243</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Night Sky Nails</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxh243</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1hxhq92</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Orange gel nails with russian manicure</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9fjupr830ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1hxhojv</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>First fresh nails of the year, I’m in love with this color palette 🥰</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xi7sscfj30ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1hxh3cr</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Geeky Graduation Nails</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxh3cr</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1hxgwlp</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>My first set of nails ever !!!</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxgwlp</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1hxgjgs</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Not my cleanest work, but definitely my favorite nail art so far!</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxgjgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1hxgfuh</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Been a while since I got red! Love it!</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3bd02jauzbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1hxgclq</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New birthday set :) </t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4ko07nntzbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1hxfvit</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Ruptured Look</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxfvit/ruptured_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1hxg2l0</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Thin nails, gel manicure, healing?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47g2pzvkrzbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1hxftdl</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Can Files Be Disinfected With HappyLight?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxftdl/can_files_be_disinfected_with_happylight/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1hxfsla</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>💅🏼</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfob4zafpzbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1hxa68x</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Second time at home gel nails</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxa68x</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1hxemj0</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>How do you remove press on nails without damage?</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxemj0/how_do_you_remove_press_on_nails_without_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1hxeu2y</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Polish? Finger cot? Something else?</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g29dzk7rhzbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1hxemar</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>New cat eye nail color. Love it!</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0a0exh72gzbe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1hxe7px</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Please help me! My nail polish peels off!</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hxe7px/please_help_me_my_nail_polish_peels_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1hxe5yh</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Painted nails in such a long time</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxe5yh</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1hxzc45</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Sassy Sauce’s “Dissimulation” is that gurrrrl 😍</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxzc45</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1hxzanu</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Wicked skittle Mani</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxy2v3</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1hxywvy</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Keeping it simple with Top of the Frock</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxywvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1hxyscw</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie - Bikini So Teeny </t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxyscw</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1hxyf45</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Loving High Voltage from my last ILNP order💜</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5lp4h9gc34ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1hxxsf4</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Pink Suede 💖</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxxsf4</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1hxxq7n</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>The color!! 💖</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oh3imnx9v3ce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1hxwdes</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Dupe for (kind of) BKL Canned Peaches and Marmalade?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxwdes</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1hxvny8</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>KBShimmer Come Sip With Us</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxvny8</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1hxvh1o</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Cirque's Rose Kaolin</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fe1emxad73ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1hxv2j8</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>ethereal purple glow</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4ivoysmi33ce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1hxuncg</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Looking for a dupe</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxuncg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1hxu7w4</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>In search of a dark dusty rose!</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxu7w4</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1hxu7ey</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Searching for a dupe of this color</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6b6rvy5iv2ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1hxu2ex</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Best quick dry long lasting top coat for nail polish??</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hxu2ex/best_quick_dry_long_lasting_top_coat_for_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1hxto3s</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I was going for "abstract stained glass" but it's giving "abstract 80's roller rink" </t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cszyfijhq2ce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1hxtd9o</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Celebrating 10 years of this sinful colors polish</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxtd9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1hxt0dv</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vibrant Multichrome polish recommendations </t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hxt0dv/vibrant_multichrome_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1hxlpe3</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wake up and polish is ruined </t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cgr60hrox0ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1hxs2g7</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the glow of moonrise - does any shade match it? </t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxs2g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1hxrtnq</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>aventurine green for good luck</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hvtic20a2ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1hxrf1q</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>swatched my HHC order!</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxrf1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1hxqulj</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Shades like House of Hades but more purple?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxqulj</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1hxqu2z</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Forgot about this in my collection </t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxqu2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1hxqmnp</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Illusionist-reversed velvet </t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9rr7wcvz1ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1hxqh76</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Update on By Dany Vianna fiasco!</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hxqh76/update_on_by_dany_vianna_fiasco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1hxqb7r</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t xml:space="preserve">On snowy days we wear pink </t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxqb7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1hxp3rj</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What brand has your favorite bottle shape? Which one do you find repulsive? </t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qedqcq4tn1ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1hxoew0</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>You know who she is</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxoew0</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1hxoe1e</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Recs for some heavy duty top coat?</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hxoe1e/recs_for_some_heavy_duty_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1hxo9w3</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>i needed a little sun in seattle:)</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxo9w3</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1hxo9lm</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is there any way to repair this torn corner of my nail? </t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofqb0jm8h1ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1hxnp4g</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone know the difference between Dany Vianna's Rosewater and it's 2.0 version? Found both on Mercari, and not sure which one to get. </t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxnp4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1hxnocq</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Finally got my polish to last more than a day!</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4z009pmmc1ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1hxnnm1</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Champagne Toast ft DSLR</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxnnm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1hxn88u</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Help!!! Nail shape?</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykjpljp791ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1hxn16f</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Matched my keyring 🐥</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxn16f</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1hxn0pu</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any MRI techs in here?? </t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hxn0pu/any_mri_techs_in_here/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1hxmp5l</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phoenix Delirium </t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxmp5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1hxmlcm</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glowy polish to save me from the snow blues </t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h560m1sd41ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1hxmc4r</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Base coat recommendations?</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hxmc4r/base_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1hxm8n7</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>💜💙 I picked up ILNP Birefringence (H) on BF and it reminded me of a polish in my collection with similar blue-purple vibes, Painted Polish Rainbow Fish Wishes. I thought they'd make a cute funky winter mani.</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxm8n7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1hxlqpq</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t xml:space="preserve">By Dany Vianna not following through on free gift with purchase promotion </t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hxlqpq/by_dany_vianna_not_following_through_on_free_gift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1hxlqa3</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another Mooncat holo - Moonflower! </t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxlqa3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1hxlp6i</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>First Time I've Painted My Nails in a while (base coat: essie strong start, ILNP You up (2 coats) and Seche Vite on top :)</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnrjzjyix0ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1hxld0s</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Nephew picked the nails</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxld0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1hxkq4i</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not sure if this is a good color for me? </t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pghzepadq0ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1hxkmsq</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>I know you think you know what shade this is…but I bet you don’t!</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxkmsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1hxkjnb</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Kitty got claws</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7fp904xo0ce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1hxk38k</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Glisten and Glow</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hxk38k/glisten_and_glow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1hxjsbd</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Flake fantasy for my first mani of 2025 💅</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxjsbd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1hxjhl8</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>back to basics 🌸🎀</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxjhl8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1hxjbqm</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>It's so hard to say goodbye...</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxjbqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1hxj8qj</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Y'all made me do it</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13g6xckbf0ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1hxilc6</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Polished for Days Lush</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxilc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1hxiest</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>CND Chic-a-delic</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0t0m0r290ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1hxi5zd</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Zero Degrees looks like a starlit glacier 🧊</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knqmctr770ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1hxhg2u</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Happy bday nails to me!</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8b6uedos10ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1hxgk8o</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Maybe the prettiest glowy pink?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxgk8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1hxgd61</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>nails for my partner’s birthday :)</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxgd61</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1hxfza7</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Does anyone else?</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hxfza7/does_anyone_else/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1hxfcin</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Chocolate Brown 🤎🍫</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxfcin</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1hxcgbt</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Magnetic suggestions</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hxcgbt/magnetic_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1hxf709</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Cuticula Cloud Cover matte topcoat - white spots?</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l11rmygpkzbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1hxf2d6</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>First post, and first lacquer in years.</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxf2d6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1hxen2i</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer - Cappuccino Cloud</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxen2i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1hxekww</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving this "my nails but better" shade! </t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxekww</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1hxehfw</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Is this a palate cleanser?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxehfw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1hxe0tz</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Press-on Polish?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hxe0tz/presson_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1hxdwk0</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First try at ombré </t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxdwk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1hxd4xj</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I took your suggestions and went for blue__ILNP Zero Degrees </t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxd4xj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1hxd008</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Out of the Goodness of My Heart - By Dany Vianna </t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxd008</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1hxc76u</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Looking for this color</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9u3hadp8uybe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1hxbzj8</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>I read a comment saying ballerina coffin nails just look like bad almonds with the tops cut off 😭😭 not sure if I should ditch this shape and just go almond?</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxbzj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1hxbfne</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Similar multichrome pigment comparison: Sassy Sauce Now And Zen velvet; Picture Polish Beetle; Noname Chrome Powder</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqrlc28llybe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1hxavyu</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Advice on getting gel overlay on slightly damaged nail</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxapqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1hx8i01</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rate the design </t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hx8i01</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1hxyn00</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Today I learned that I hate doing 90s nail art</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnlnncb264ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1hxw6dr</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Electric blue 🥰</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/89lnonsle3ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1hxvxhu</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Rosemary’s Baby 🕯️</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxvxhu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1hxuv10</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t xml:space="preserve">✨ Dino 🦕 </t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yathjwtl13ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1hxtyzx</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Cable knit pattern - couldn't narrow down the colors!</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3qt5l4dt2ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1hxsvqu</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Need nail ideas for laneway festival!!</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hxsvqu/need_nail_ideas_for_laneway_festival/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1hxss5x</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>crystal depth effect tutorial</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iukjhmghi2ce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1hxsc1m</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Painting Ellen from Nosferatu for a Nail Set 💞🫶🏼</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0vzerwfe2ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1hxqt3x</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should they be Mary Janes? I love </t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8yr91dd12ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1hxqmuk</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink Pony Club ✨ 🦄 </t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxqmuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1hxq6ae</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Need some inspo for a set!!!</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hxq6ae/need_some_inspo_for_a_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1hxpa5n</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>My fiery start of the year</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vehb8677p1ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1hxo88e</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Fallout 4 inspired nails☢️</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxa8l1zxg1ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1hxo50z</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Custom Apple set</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxo50z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1hxmw8o</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Something simple :)</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vcnme0oo61ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1hxmfse</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>New year, new nails!</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0g7eo86831ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1hxlisb</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spider set!! Gothic kinda </t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxlisb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1hxjkua</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Birthday set on myself 🎈</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxjkua</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1hxjjv5</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Irn Bru Nail Set 🧡 For Fun &amp; Giggles </t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jx1w91mh0ce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1hxirng</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Yesterday✨💜</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxirng</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1hxfdes</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Dark Victorian set</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hxfdes</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1hxem8i</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt at graphic nails. I want to get better! Critiques would be super appreciated! </t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jh30gt1gzbe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1hxasf5</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Dreamy pastel vibes with touch of floral elegance  🌸✨</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ieodabhieybe1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jan 11 08:09:32 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_12.xlsx
+++ b/data/collected_data/2025_01_12.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1059"/>
+  <dimension ref="A1:C1264"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18443,6 +18443,3491 @@
         </is>
       </c>
     </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1hyrb01</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>That's my style today</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kikvqyfbobce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1hyr5xp</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Why is there that line in the white part of my nail?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vslwprakmbce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1hyr361</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Do you think it is a very dangerous length?</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwz1dmbjlbce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1hyr0fk</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting my nails done! </t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyr0fk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1hyqn3l</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Absolutely obsessed with this wintergreen sparkle ✨</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/9ru63Dh.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1hyqhxl</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>I have questions and need help please🥹</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fp59wacmdbce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1hypxkp</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did sculpted gel overlay on my natural nails. </t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z218lrlm6bce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1hypder</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Natural nails idk if i should switch to almond shaped</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bq07gohyzace1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1hyo6mx</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what’s this? </t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyo6mx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1hyo5ms</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>What’s going on?</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyo5ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1hyp35g</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>My nails. Made by me. Pretty good for me 💕</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyp35g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1hyowxe</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>New to the sub, first set of the year!</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyowxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1hyojlp</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>First set of 2025</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/deyoamevqace1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1hynnbi</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got home and didn’t like them </t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4isbk8jhace1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1hynjov</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails 💅🎁 </t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bni85p9igace1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1hyn01d</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>nails advice!!</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/33elftb2bace1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1hylxj0</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set of the year </t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ky3k99vr0ace1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1hymv7t</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bright white nails I did on myself </t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hymv7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1hymhv8</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail bed lengthening? </t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hymhv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1hymgxk</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>First two nail extensions!</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hymgxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1hymeb2</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Keeping pretty natural nails without polish or buffing? </t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hymeb2/keeping_pretty_natural_nails_without_polish_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1hym3m1</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Trying to grow my nubbin nails longer and seek the wisdom of anyone with long nails 🙏</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3smjrgne2ace1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1hylvxp</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Got gel-x for the first time!</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5tyeypc0ace1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1hykx8s</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Should I get them redone?</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0mvjtxcr9ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1hyl809</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Nail shape suggestions</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyl809</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1hykuja</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>What kind of acrylics should I get for my first time?!</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hykuja/what_kind_of_acrylics_should_i_get_for_my_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1hyl37p</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/stzzur1xs9ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1hyktdf</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Pink mismatch nail art! (I’m still trying to improve on my line work)</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mbclvveq9ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1hykrwk</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Help with electric file</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hykrwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1hykj6u</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>growing out my rings of fire before i start my long natural nail journey</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/elbm8h3vn9ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1hykc6y</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails cut down yesterday </t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hykc6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1hyjrnl</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>What shape acrylics should I get?</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyjrnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1hydhhe</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails keep splitting :( help! </t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hydhhe/nails_keep_splitting_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1hyka3g</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me the best?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyka3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1hyeec7</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cold inspired nails </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyeec7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1hyg7vw</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Is my nail shape coffin?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyg7vw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1hyie02</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>press on related accident left me with split nail how can i grow this out // help it heal</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/re476mnc59ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1hyiqaw</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Question about nail bed dip..</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyiqaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1hyh9m3</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>does anyone know what these ridges on my nails could be from?</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyh9m3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1hyhpwk</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>natural nails always split with gel polish???</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6btwlhswz8ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1hyjzut</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it that serious ? </t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y14rxn83j9ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1hyjx53</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i didn’t even know cat eye existed. my nail tech fr the picasso of nails </t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pafl5qsei9ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1hyjgfa</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first extensions </t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xx5aslqde9ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1hyj9k9</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>almonds transformed my hands 😍</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyj9k9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1hyj544</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Graduated Nail School Today :-)</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2044emsb9ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1hyibmh</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Love my new set</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ky938u8v49ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1hyi923</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help with best shape &amp; length nails for my hands. </t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyi923</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1hyhw82</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Pretty in Pink 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ppto4dzc19ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1hyhix3</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Black with silver fires 🖤🩶 🔥</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nflvg92ey8ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1hyh6a8</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black and silver glitter </t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyh6a8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1hyh676</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>which shape looks best?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyh676</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1hyh1cl</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink Aura Nails 💅 </t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyh1cl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1hygq59</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A new set </t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/814q4dw1s8ce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1hygph9</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Help - crack in nail</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obr7uqjwr8ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1hygm9r</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Help me</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6lzix07r8ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1hygfsd</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Sad day, took off the acrylic nails and have natural nails!</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xphrrozrp8ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1hyg7hm</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Gel extension length</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hyg7hm/gel_extension_length/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1hyfxp1</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Yay or nay??</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jjj54zvsl8ce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1hyfuym</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm stopping biting my nails and they look like this: </t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zligod2bl8ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1hyfosi</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Marble(ish) blends + gold</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyfosi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1hyfiox</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Early 2000s 🫠</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyfiox</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1hyfg3y</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Trying new color 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h36j8bm1i8ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1hyec7d</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>New to press-ons - are tabs good?</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hyec7d/new_to_pressons_are_tabs_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1hyeda9</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Adding a curve?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyeda9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1hyfck9</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>my new manicure for these days</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ef4k2gi5h8ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1hyfb05</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>My new nails style</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyfb05</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1hyf04x</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set New length </t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfiqwnfme8ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1hyemnq</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Questions for techs working in a salon!</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hyemnq/questions_for_techs_working_in_a_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1hyel6d</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>New nails set for my birthday coming up</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyel6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1hyecox</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Wanted a little break from red 💗</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyecox</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1hydyn1</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Does gel weaken natural nails?</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hydyn1/does_gel_weaken_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1hydult</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>My fav nails ever 🦴🖤</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hydult</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1hydpqk</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>How to help gel polish last</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hydpqk/how_to_help_gel_polish_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1hydhwl</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Valentines nails!</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hydhwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1hydf9c</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>In love with this combo - cherry red, plus silver glitter top with colourful flakes</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1w618vct28ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1hydbuw</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>New set 🥰🩷</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egf9qp4528ce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1hy99eb</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are my cuticles irreparable?! </t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/parm9qi187ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1hycdjg</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>amateur nail artist trying to open commissions, unsure of how to price fairly</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hycdjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1hyar48</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why do my pinky nails curve downward? </t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lo26ls32j7ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1hyblsn</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>First time doing my own nails with hard gel!</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyblsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1hybo15</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone else’s nails naturally grow in as different shapes? </t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hybo15/does_anyone_elses_nails_naturally_grow_in_as/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1hybrlv</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Help with ombre technique (it takes me so long)</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hybrlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1hybqpe</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>🥺</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8aba5dlcq7ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1hyblzf</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Growing nails</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oiuetbddp7ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1hyb8jw</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>First Set of 2025</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulplqdjlm7ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1hyb0i7</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Smorgasbord nails</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9nh65ccyk7ce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1hyaroz</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Pop off sets as press ons</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hyaroz/pop_off_sets_as_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1hyacrc</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">January blues </t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ql4b3y46g7ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1hyaa5u</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i listened to all of you and chose a shorter almond </t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyaa5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1hy9v7b</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Current ombré nails. What should I do next?</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5takg2jc7ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1hy9sq8</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spicy nail set </t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy9sq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1hy9js7</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Icicle Nails insipired by u/Ok-Plant888</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy9js7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1hy9e3v</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Gel-like nail glue that isn't gel?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hy9e3v/gellike_nail_glue_that_isnt_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1hy96v4</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>MOONCAT - Green Eyed Monster</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvi933xh77ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1hy8441</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love my new nails! </t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ouons7iz6ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1hy51me</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>tips for chunky gel nail removal at home?</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy51me</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1hy7c2r</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Subtle and elegant, love this set</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mq33eowgt6ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1hy6t8g</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">do square nails suit me? i’ve always done short tapered square and i have tried oval/almond and absolutely hate it on my hands but if y’all think i’d look better with oval/almond i’ll maybe try it again.. ugh 😔 i love oval/almond on others though! </t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy6t8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1hy658a</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Lights Lacquer The Night Before</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4o42l1b4k6ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1hy5qo5</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Do you think these have another week on them? Or should I go in for a fill this weekend?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktoc9jlqg6ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1hyqhor</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Loving this and the formula 😭</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjw7m2djdbce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1hyp7yk</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Rockin’ Rock ‘N Roll</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyp7yk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1hyoycb</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>I fear I have a type (doing my nails for the swamp 🐸🐊🪲)</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgkxmuk8vace1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1hyouu4</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Been watching a lot of Planet Earth…</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tk0ic4s6uace1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1hyop3l</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>How to make an awful neon formula work?</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hyop3l/how_to_make_an_awful_neon_formula_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1hyo4hj</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Flicker</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyo4hj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1hyo40q</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>winter nails ✨❄️🩷 (non-gel)</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyo40q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1hynrwm</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Holo alert</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/482mohiuiace1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1hynm5f</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>linear holos. always and forever.</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hynm5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1hynhle</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gomez. and morticia. always. </t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jjvlqxkface1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1hyndap</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In January we wear untrieds! </t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyndap</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1hymhtz</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>My First Frankenpolish!</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hymhtz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1hymhq4</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>My First Frankenpolish!</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hymhq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1hymh7z</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Phoenix Indie - Where to Purchase</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hymh7z/phoenix_indie_where_to_purchase/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1hymf9l</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Death Valley Nails gloopy formula - anyone else?</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hymf9l/death_valley_nails_gloopy_formula_anyone_else/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1hymegk</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ever Come Across a Bottle You Forgot That You Bought? </t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hymegk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1hym0rl</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Are there any benefits to putting a matte topcoat under anything? (Like under a color or under a glossy topcoat?)</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hym0rl/are_there_any_benefits_to_putting_a_matte_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1hylzhs</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Nail newbie</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hylzhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1hylr1u</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They look so… organic? </t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hylr1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1hylqyu</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They look so… organic? </t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hylqyu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1hylpd5</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Regarding call out posts (bad experience with a brand)</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hylpd5/regarding_call_out_posts_bad_experience_with_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1hyl8i0</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Empties &amp; Plan to Pan (Project Polish) </t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyl8i0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1hyl0nz</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Something pretty for between manis?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hyl0nz/something_pretty_for_between_manis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1hykvtd</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>What kind of acrylics should I get for my first time?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hykvtd/what_kind_of_acrylics_should_i_get_for_my_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1hykrcj</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>What’s a combo you love so much you’d wear it to your grave?</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hykrcj/whats_a_combo_you_love_so_much_youd_wear_it_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1hyk2qm</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>I can't believe I almost redid this set</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyk2qm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1hyjvu7</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>A Comet’s Tail</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ookbbdw2i9ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1hyjeqr</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t xml:space="preserve">January garnet nails </t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyjeqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1hyike8</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">By Dany Vianna response and original emails in order for context. </t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyike8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1hyigrv</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Is this a bad gel paint job, or am I just being picky?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyigrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1hyia4s</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t xml:space="preserve">help me narrow down my color4nails cart! </t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0y27rwld49ce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1hyhwt1</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Power Surge💚</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/at4rfcfg19ce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1hyhl0e</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Ridge filler that dries clear (or mostly clear) without PVB?</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hyhl0e/ridge_filler_that_dries_clear_or_mostly_clear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1hyhg43</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Suggestions please!</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcwo5hpqx8ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1hyh14l</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Best matte top coat?</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hyh14l/best_matte_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1hygsm2</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>ILNP Quicksand 😍</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hygsm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1hyg7yi</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Winter blues</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5v1fig2o8ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1hyg27c</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Overcast collection in its natural habitat </t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyg27c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1hyg0gw</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Devil’s Ivy 🌱</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyg0gw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1hyeydt</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Mani 2/52 Done!</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyeydt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1hyeipz</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Most hyped flakies, multichromes, opalescents?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hyeipz/most_hyped_flakies_multichromes_opalescents/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1hyehpy</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Pink Sparkles 💕✨</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyehpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1hy8ulf</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pink to break up the wa grey </t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4251ycqw47ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1hye8gi</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My January reset nails </t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mymtajs88ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1hye883</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can’t decide if these nails look classy as hell… or like poo 💩 </t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hye883</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1hye2gu</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Polish Tracking Spreadsheet </t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ybmtvol78ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1hydtwv</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🩵💎💙 I layered two blue shimmer polishes, I’m obsessed </t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hydtwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1hydoub</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Colors to make hands look less red and crusty post chemo?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15g0ll5s48ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1hydb5r</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>lightning in a bottle ⚡️</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hydb5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1hyd3d9</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>atomic polish - bioluminescent</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyd3d9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1hycfka</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Getting the hang of magnetics</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wobt8l9cv7ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1hyceya</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Hypnotizing shift</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5m9miaa5v7ce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1hybym0</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>What happened to all the other versions of OPI Nail Envy?</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hybym0/what_happened_to_all_the_other_versions_of_opi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1hyb5n6</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Winter vibes for this shade are impeccable ✨❄️🩵</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyb5n6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1hyb1zr</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Is there a trick to getting better opacity out of Pacifica nail polish?</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gylw7tw9l7ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1hyaqja</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>ILNP Bluebell 😍</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aldcs7wui7ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1hyaoud</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Venom Really is Something Special! 🐍</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y10dddpki7ce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1hyak1b</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Most Problematic Brands According to Sub Discord</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/W5W4jTc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1hyab57</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>I reckon this is as long as my nails go before butting heads with my guitar 🎸</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wn2irkdtf7ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1hya8ru</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Gracie &amp; Jay Order Just Came!</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rj3c4xicf7ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1hya7jk</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Unusual discussion - has anyone ever tried to make their own polish or nail stain?</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hya7jk/unusual_discussion_has_anyone_ever_tried_to_make/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1hya33p</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Nails I Did This Fall, Couple Months Late</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8ll6ad7e7ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1hy9x2w</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Tried magnetics for the first time and I'm in love!!</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5g7vc7lc7ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1hy9uz9</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>ilnp Blowing Bubbles love</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lzmrqp3hc7ce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1hy9t8c</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Emily de Molly - Distance to the Sun or Never Found It?</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hy9t8c/emily_de_molly_distance_to_the_sun_or_never_found/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1hy9mok</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>At-home chrome for my b-day nails</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy9mok</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1hy9m3z</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Damn Holiday Sales! *shakes fist*</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5salcpona7ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1hy9joo</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>It's like a dream~</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy9joo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1hy9bid</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mystic / Etherial Neutrals, But Warm?  </t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hy9bid/mystic_etherial_neutrals_but_warm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1hy9b4a</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Boa Constrictor (Mooncat) is so underrated</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy9b4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1hy97y5</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>MOONCAT - Green Eyed Monster</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2a777j1r77ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1hy95pc</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>If you wanted opaque, workable shimmers…</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy95pc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1hy8s7p</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are your most loved deep/dark blue polishes? </t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hy8s7p/what_are_your_most_loved_deepdark_blue_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1hy8lqd</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Does essie hard to resist need a base coat on top?</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hy8lqd/does_essie_hard_to_resist_need_a_base_coat_on_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1hy8jwx</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>PSA if you wanted Cirque Spa Water!</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy8jwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1hy8c1t</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Comparison Request: Lust for Vengeance vs Fair Isle?</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy8c1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1hy837v</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thoughts on new Phoenix? </t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/finahpkbz6ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1hy7qzr</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>RIP 😭</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy7qzr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1hy6wa9</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🩶 Such a Farse 🩷 </t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sormxeq2q6ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1hy6p16</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>What are your favorite brands for cremes? 🍦🍨🥯</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hy6p16/what_are_your_favorite_brands_for_cremes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1hy6p00</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>What flatter brand of press-ons would you recommend?</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hy6p00/what_flatter_brand_of_pressons_would_you_recommend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1hy5jfc</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Really wanted to love this one on me but my skin tone had other ideas :(</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy5jfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1hy52wr</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Was trying to embody an icy morning with this skittle </t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1q5xudg2b6ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1hy4s0s</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Snow Much Fun! ❄️</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy4s0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1hy4nfe</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Which polish brands are on your no-buy list and why?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxeferc876ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1hy4g49</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Birthday girl on my birthday</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy4g49</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1hy3ygx</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Brown bling! 😍</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gn62dqtk06ce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1hy1z84</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>HHC Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hy1z84/hhc_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1hypjve</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Forest green marble nails </t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hypjve</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1hypcta</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One of my favorite sets from my nail tech, Diana from Toda Beauty. These are from last Halloween </t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hypcta</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1hyp3kd</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Custom nail art prices</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hyp3kd/custom_nail_art_prices/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1hyl9ez</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Birthday set!</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qarisihu9ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1hyklwn</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Advice needed!!</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hyklwn/advice_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1hykl2p</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>What do you think? I'? New🥰</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clbkplhdo9ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1hyip8r</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Strawberry Kitty Nails</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyip8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1hyikma</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how to make chrome look better </t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwxdw1oz69ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1hydkkb</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>💖</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2951fav38ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1hybp10</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Help with ombre technique (it takes me so long)</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hybp10</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1hyaryg</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Flowers &amp; pink cat eye press-ons I did for my mom 🌸</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1fq3068j7ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1hyah3b</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Je fais mes ongles moi même ;))</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyah3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1hy7q5f</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Painted my left hand, didn’t like it and went a completely different direction with my right😅 Thoughts? In a creative rut right now.</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwzk4tmcw6ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1hy2qsp</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A few summers ago! </t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjfxivhnn5ce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1hy1sdb</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Valentine teddy bear nails ❤️🐻</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy1sdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1hy1nqe</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>How do you handle having charms on your nails?</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hy1nqe/how_do_you_handle_having_charms_on_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1hy0a12</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Got my nails done in Japan!</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hy0a12</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jan 12 08:09:16 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_12.xlsx
+++ b/data/collected_data/2025_01_12.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1264"/>
+  <dimension ref="A1:C1480"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21928,6 +21928,3678 @@
         </is>
       </c>
     </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1hzi2bb</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Fav short set</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emaqzg7gtice1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1hzi12j</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>One of my favorite sets</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzi12j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1hzhx62</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Press ons I got for my daughters birthday/first set of the year</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bb703xcmrice1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1hzh0pq</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Awful $80 set 😥</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzh0pq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1hzgqfm</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Getting back into stamping!</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hp692ekgcice1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1hzh1py</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love me a cat eye! </t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8uxcxgibgice1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1hzgxti</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>any spring nail design suggestions?</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hzgxti/any_spring_nail_design_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1hzgwfh</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic stiletto!!! </t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mweva1oieice1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1hzfr0g</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Instantly thought of Howls moving castle! </t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzfr0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1hzfqua</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>💙✨</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzfqua</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1hzfpea</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>My nail tech slays every single time</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pwn0j1h30ice1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1hzfjv4</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>First time getting gel-x - what’s wrong here?</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzfjv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1hzfbdo</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>How to remove press ons with NYK1 glue??</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hzfbdo/how_to_remove_press_ons_with_nyk1_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1hzff2l</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>first cat eye 🔮</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrz9k8l9xhce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1hzf9ro</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Can you see a difference?</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzf9ro</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1hzeldp</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Nails so thin after having gel x for two months. Should I get a gel manicure or keep them natural?</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hzeldp/nails_so_thin_after_having_gel_x_for_two_months/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1hzemoj</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>I walked out of my nail salon without tipping</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hzemoj/i_walked_out_of_my_nail_salon_without_tipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1hzejeq</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>First time doing my nails using a gel builder kit.</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzejeq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1hzehgk</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>holo taco everything is pine</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hzehgk/holo_taco_everything_is_pine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1hze9z6</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Dark Violet Smoke?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/giwqgt5blhce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1hze0po</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>What shape is best for my nail bed?!</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4l8dtbfqihce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1hzdpqi</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>My nail tech suggested a cat eye French mani and I ain’t mad 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zk4ngy7ofhce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1hzdm6j</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Russian manicure </t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hzdm6j/russian_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1hzdhi6</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Wanted something subtle but fun.</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5l0to9tfdhce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1hzcuai</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>I hate my nails right now 😭</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzcuai</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1hzd291</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Just sharing my January snowflake nails!</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7uvcy0c59hce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1hzcv4c</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Mismatch Funky Set 🎨</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzcv4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1hzctpf</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>first time getting my nails done.</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hf8rjmly6hce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1hzctcp</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Snowflakes ❄️</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lypjmz3v6hce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1hz2fl1</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Toenail halfway broken</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2tge2kt3sece1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1hz9nt3</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! How do I achieve this 3d/texture Rococo Style gilded frame look? </t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz9nt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1hza2ds</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>How do I make my nails stronger?</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hza2ds/how_do_i_make_my_nails_stronger/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1hzaivz</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nail inspo 💅🏼💕</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zh9xwoymlgce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1hzcmfw</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>A little blue sparkle</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3t2x2k05hce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1hzbwa3</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HELP: desperately trying to rehab my peeling nails but getting daily snagging, pulling, scraping despite best attempts at being careful  </t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzbwa3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1hzci6s</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>🩷</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpsbnt4v3hce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1hzbqg0</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Does anyone know why my nails do this?</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzbqg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1hzcg1l</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">don't have a nail stand, but we are making do!! (tape and a phone stand, lol) </t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/evohnhsz2hce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1hzbjkr</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Broke a piece off my nailbed what to do</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hzbjkr/broke_a_piece_off_my_nailbed_what_to_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1hzc8sb</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">quack quack </t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9nw1dng91hce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1hzc883</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Is it possible to fully cure gel polish with the handheld uv light (those portable ones)</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hzc883/is_it_possible_to_fully_cure_gel_polish_with_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1hzbzgi</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set of Press ons! </t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8yoabmvygce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1hzbtmh</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Sticking to almond shape!</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7h3tp9xdxgce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1hzbon4</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>New set! I am in love with them!</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxuedod3wgce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1hzbj7b</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>polka dots :3</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzbj7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1hzbi0a</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>lunar new year! 🍊🧧</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzbi0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1hzb3k6</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PolyGel set </t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzb3k6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1hzak68</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does this color look okay? I wanted a red-orange but it’s a bit more orange than I thought it would be. </t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0w1ul3wxlgce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1hzajxy</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Tried my hand* at growing out my nails..</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l69uqlmvlgce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1hzafpt</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>my nail tech blesses me every time</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pf52sxmvkgce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1hzab45</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>My nail tech is so beyond talented. I’m speechless😭✋🏻</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aic07v6sjgce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1hz9zye</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>january nails ❄️</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz9zye</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1hz9yyg</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Some winter glitter</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz9yyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1hz9tss</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some of my recent work. </t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz9tss</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1hz9rdg</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>First time doing my nails, advice?</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptuv1q75fgce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1hz9qmt</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>What does it mean to apply a press on at an 45° angle?</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hz9qmt/what_does_it_mean_to_apply_a_press_on_at_an_45/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1hz9ozs</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>love a middle finger star.</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xh13y1rkegce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1hz5b3q</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black cherry </t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz5b3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1hz962v</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>is it okay to do a gel-x set over thin nails?</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hm3xx74agce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1hz5sy6</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Gel manicure - what am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hz5sy6/gel_manicure_what_am_i_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1hz6c6b</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>What nail shape would this be considered. Photos by @margsandmanicures on tik tok</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz6c6b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1hz8kft</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetle gel </t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hz8kft/beetle_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1hz8348</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>silver team</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz8348</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1hz8114</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Felt sparkly today </t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9py0fan0gce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1hz80ua</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Poly gel nails</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xj2apwl0gce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1hz7zy8</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Pls rate nails that my auntie did, (Don’t judge back ground was at hair salon 💔)</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mu1r8uvd0gce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1hz7r5e</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Hi! I am a beginner nail tech and I recently bought every single thing I need to start doing nails, but I need some good acrylic brush recommendations.</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hz7r5e/hi_i_am_a_beginner_nail_tech_and_i_recently/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1hz7jln</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Press on nail help</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gmp9dwnqwfce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1hz7566</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Working my way up to long stilettos</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz7566</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1hz6ugl</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Tried something Spooky Cute</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hz6ugl/tried_something_spooky_cute/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1hz6hh7</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time acrylics </t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kahvquobofce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1hz5wrf</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>I really love how this turned out💛✨️</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz5wrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1hz5q30</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Learning how to do my own nails</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hz5q30/learning_how_to_do_my_own_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1hz5bnz</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Might be my new go-to!</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xsfvdpyefce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1hz5b04</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set for my trip next weekend </t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/an9bk0otefce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1hz59d3</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Gel x vs acrylic for a beginner</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hz59d3/gel_x_vs_acrylic_for_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1hz4twx</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Blooming gel animal print</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvbadvf0bfce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1hz3u3l</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Cuticle cutting tips?</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hz3u3l/cuticle_cutting_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1hz44gg</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>What do you think about black nails?</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hz44gg/what_do_you_think_about_black_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1hz3x8u</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>First attempt at cat eye on natural nails</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz3x8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1hz3viy</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>felt cute ❤️</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz3viy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1hz3tnr</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Wanted a simple look, went with navy blue glitter</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz3tnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1hz3t77</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Biab designs&lt;3</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz3t77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1hz3mus</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Low humidity fluid art just hits different </t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0tx6zvj1fce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1hz30uz</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Experimenting with chrome isolation</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tbhswxyrwece1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1hz2zek</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got nail tips (gel x) for the first time and I no longer know how to use my hands </t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqhrj0ugwece1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1hz2szt</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>first time with acrylics</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz2szt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1hz29r3</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Nail tech used an Orly clear polish with a cold rim and kind of a pink floraly print on the handle, does any one know that this is called?</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hz29r3/nail_tech_used_an_orly_clear_polish_with_a_cold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1hz23yz</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Nosferatu could never 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4euv7rkpece1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1hz20oe</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Square hue-times square </t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz20oe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1hz1xox</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>🦜 Parrot Nails 🦜</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwpqgjk8oece1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1hz1vdm</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Nails poly gel</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wea0huiqnece1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1hz1nbj</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>nail pens for gel?</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hz1nbj/nail_pens_for_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1hz1idm</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Current Nails </t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmx4zdo0lece1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1hz0t06</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>nails are jewels not tools 💅🏻✨</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz0t06</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1hz1bnl</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you remember when this material on nails became fashionable? </t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ma35isqjjece1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1hz12bz</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel Stickers </t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hz12bz/gel_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1hz10vj</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Advice</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz10vj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1hz0sue</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>My vacation nails after a week abroad. Forgot my cuticle oil 🤦‍♀️</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2janozpgfece1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1hz0on9</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Deep red vibes ♥️</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0x8n6rjeece1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1hzhhgo</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>ILNP Amber</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzhhgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1hzh87m</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Two different glitter looks</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzh87m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1hzgy15</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Experimenting with lace style stamping plates</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pd982t82fice1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1hzg2yf</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dropped the entire clean up brush in acetone and now it’s milky white… what do I do with the rest of the liquid 🤦‍♀️ </t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3nyp6ism4ice1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1hzfpax</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>January HHC by Sassy Pants</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzfpax</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1hzeom2</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Help! QDTC causing polish to peel up</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzeom2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1hzel5e</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Looking for other lacquers like Mooncat's Fields of Lavender (non-magnetics welcome)! I am just in love with that "orangey red first" glow.</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3t1d2zq7ohce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1hzdrjn</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Starrily Quartz Crystal 💎🔮</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1fgptj7ghce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1hzdg1h</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>If I could only use one shade for the rest of life, I'll always choose red</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzdg1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1hzda1l</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Well, I blame you guys</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ai9407fbhce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1hzda0h</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>First thermal - such a rad transition!</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzda0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1hzd745</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Obsessed with ILNP Pink Suede</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jeq2uiblahce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1hzd2i3</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Found my perfect opal-like combo </t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6bq3veyc9hce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1hzcmzd</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>A little sunshine 🌞 in this dreary winter</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzcmzd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1hzck6x</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Got a bit excited for my first ILNP order 🤭</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzck6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1hzcjkb</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>💜Glitter Jelly mani💜</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzcjkb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1hzch6g</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>I'm itching to buy a new pink polish, give me your favorite pink polish(es) please!</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hzch6g/im_itching_to_buy_a_new_pink_polish_give_me_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1hzcdku</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any other football laqueristas out there? Let's go Ravens!! </t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2pvx4y2k2hce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1hzc0wb</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>I think this is the most interesting mani I've ever done.</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzc0wb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1hzbo4u</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Mooncat’s Memento Mori - similar to Cirque Colors Soleil or another equivalent?</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hzbo4u/mooncats_memento_mori_similar_to_cirque_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1hzbidb</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Lumen's Sagittarius Mystery Bundle and Glass Stars Ooops Batch WARNING: Bad nails, bad lighting, bad photography, bad editing, etc.</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzbidb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1hzbh6e</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Multichrome Skittle Supremacy!</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzbh6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1hzb2ef</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Gel/regular sandwich</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hzb2ef/gelregular_sandwich/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1hzb1ek</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Multichrome skittle! I’m in love with these polishes.</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzb1ek</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1hzaub6</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SOS: held hostage by peeling brittle nails </t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzaub6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1hzas9u</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Dupe for discontinued Orly</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99u4qwxvngce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1hza7uq</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FIRST ILNP order! </t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hza7uq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1hza0a4</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>I cannot decide how I feel about this color. It's certainly unlike anything else in my collection!</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hza0a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1hz9761</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kbshimmer Super Star topper request </t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hz9761/kbshimmer_super_star_topper_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1hz87xo</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nourishing, non-hardening base coat </t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hz87xo/nourishing_nonhardening_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1hz87hx</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Anyone able to compare HT Devil’s Advocate to Cracked Cordially Invited?</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hz87hx/anyone_able_to_compare_ht_devils_advocate_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1hz7zps</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s your favorite ‘my nails but better’ polish? </t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hz7zps/whats_your_favorite_my_nails_but_better_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1hz7vah</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>First January Mani 💜🔥</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz7vah</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1hz79bx</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Doing my part to mitigate harm: By Dany Vianna's "The Willis". Further discussion in comment below.</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz79bx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1hz73ih</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Influence Me! - Zoya</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hz73ih/influence_me_zoya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1hz6vss</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Opal in the sun</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz6vss</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1hz2b1j</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>First time prepping my nails properly</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz2b1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1hz6g2j</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Advice for shaping nails?</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz6g2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1hz6aw2</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Pahlish - Mushu ❤️🐉</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz6aw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1hz6a5v</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>“Eccentric” by Sassy Sauce🤯</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz6a5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1hz5wzy</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>My first time trying solar polish</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz5wzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1hz5sfm</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Cirque Colors -Black Swan</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izah3odpifce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1hz5q85</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>I'm not too late to the velvet nail trend, right?</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i3a9w8e2ifce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1hz5lv6</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>noooooooo</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5h9m1hi9hfce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1hz5j91</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Cracks in top coat?</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz5j91</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1hz5aty</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>I love this color</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sszt17sqefce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1hz56sj</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>pink nails &amp; supernatural roleplays 💅🐉</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz56sj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1hz560k</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Glowy shimmers are my favorite</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz560k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1hz51ew</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Cirque colors bright side</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz51ew</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1hz4v6p</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using nail stickers! </t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz4v6p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1hz4qwv</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Me: Maybe it'll look better finished! Spoiler: It did not 💀</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz4qwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1hz4pjf</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>PFD Black Friday GWP Dupe Request 🙏💖💚</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8r636ir0afce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1hz4ivq</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>baby’s first ILNP purchase. excited doesn’t even begin to cover it 🥹💞✨</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz4ivq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1hz485l</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Los Angeles Wildfires: Brand Donation Megathread</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hz485l/los_angeles_wildfires_brand_donation_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1hz3w60</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Almost perfect </t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nosua7jl3fce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1hz3nnp</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Tan Shimmer Nudes?</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz3nnp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1hz2zde</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Brunhilda</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz2zde</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1hz2mv4</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Freudian Slip by Mooncat</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcxkmjzotece1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1hz2da3</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Swatches - Numerous</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz2da3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1hz27gd</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>The Queen of Pruglies</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz27gd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1hz23do</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Too early for valentines?</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hz23do/too_early_for_valentines/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1hz1vj0</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>I looove sheer polishes! Are there any like these but in a deep/cool green?</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz1vj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1hyohwj</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>I need advice</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hyohwj/i_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1hysiwr</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>do i remove nail varnish thats on my broken nail?</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hysiwr/do_i_remove_nail_varnish_thats_on_my_broken_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1hz1pdk</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>Are these squoval, or oval?</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz1pdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1hz1esl</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Favorite Indie Muted Pastels (any finish)?</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hz1esl/favorite_indie_muted_pastels_any_finish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1hz1epn</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Thoughts on the By Dany Vianna Incident</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hz1epn/thoughts_on_the_by_dany_vianna_incident/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1hz1dyx</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/jrvPbQ6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1hz0u80</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>looking for your holy grail glossy top coats!</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hz0u80/looking_for_your_holy_grail_glossy_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1hz0u6l</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second mani of the month </t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz0u6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1hz0b74</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Suncrusher by Nevermind</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hz0b74/suncrusher_by_nevermind/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1hz01dq</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>Anyone know of a topper like this, but gold glitter instead?</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjfphxcj9ece1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1hyzgvu</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Which one?</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9iz4xp35ece1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1hyyzww</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Polishes I made and wore so far this year</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyyzww</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1hyyzgc</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>is it too late to share my Christmas nails??</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mp6ptlo41ece1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1hyyspv</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Advice for hormonal changes and nail care</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hyyspv/advice_for_hormonal_changes_and_nail_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1hyy4vu</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>Clionadh</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hyy4vu/clionadh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1hyy0m9</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>Black and gold theme</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyy0m9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1hyxp8b</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Questions about making frankenpolishes (caption)! Pics are some I’ve made myself… I almost exclusively wear blue/green/teal but I’m trying to force myself branch out lol</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyxp8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1hyxed0</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Torrent </t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gd6gfp4sndce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1hyws1z</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Elphaba-inspired look!</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0exnvss7idce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1hyuv45</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Olive greens deserve more love! 💚🫒</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyuv45</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1hyu5y3</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>ILNP Songbird 🕊️</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyu5y3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1hyt8w4</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Dupe for Hard Candy Frigid ?</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbvg357fecce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1hyt1s7</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>daybreak disappointment no more</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rm0posuqbcce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1hysyhw</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>Sheer polish help</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q40f39jjacce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1hyst4n</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hand painted bows by me! (__kmnails) </t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kojk7blk8cce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1hys272</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>I blame you all :)</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hys272/i_blame_you_all/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1hyrtww</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Made my first big indie purchase and so in love!  Here’s a few of my faves.</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hyrtww</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1hzgrqg</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>Kawai nails!!!! 😍</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7kc6e4wcice1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1hzfsyr</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some recent practice </t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzfsyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1hzetf8</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>First real time of nail art ( how bad are they)</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l47eb7yvqhce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1hzeo7l</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>My favorite set for ages</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzeo7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1hzbpz4</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>Pink or blue? 🙈 💕💙</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzbpz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1hzb0o3</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opals in the sun </t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzb0o3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1hza1f7</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>No gel</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpx7s9qkhgce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1hz9oid</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! How do I achieve this 3d/texture Rococo Style gilded frame look? </t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz9oid</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1hz8y87</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>Press ons!</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oo6s8w7a8gce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1hz8ruw</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>How can I fix this?</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24foh4mt6gce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1hz8q64</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Creepy Cute Set 🦇</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz8q64</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1hz80gq</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Clown Nails by Nicole.Nailartistry</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zt3rh9xc0gce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1hz7cj4</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>Flower nails with gold flakes</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz7cj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1hz7beb</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>y2k nails (beginner)</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rhg4p7yufce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1hz70ss</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>Type O Negative</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz70ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1hz5v5n</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>I really love how this turned out💛✨️</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz5v5n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1hz4y4p</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>Blooming gel animal print</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hdmkesbybfce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1hz4ilu</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>Snow Queen Nails</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6w3z3qh8fce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1hz4fup</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>Looking for more art gels…</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz4fup</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1hz2qpb</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t xml:space="preserve">firs time using stamping, how is it? </t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nb0fdm18uece1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1hz2iqw</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>Neon glow nails</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hz2iqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1hz1y3e</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>🦜 Parrot Nails 🦜</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/memuflgboece1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1hyzdaj</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>Animal print  , in love this set made by me ✨</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rsi9hja84ece1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1hyxc4p</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nature 🍂  made today by me </t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofnkcos7ndce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1hyx17c</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>cute nails 💗 by me 🤗</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7x85l56kdce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1hyv5kf</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>Does someone know how to une nail art powder please ?</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2e7v0e82dce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1hytcol</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>🦷 nails</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hytcol</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>